<commit_message>
Updated w/ updated mothur data: phyloseq object, alpha div
</commit_message>
<xml_diff>
--- a/figs/Table_S1_SquirrelInfo.xlsx
+++ b/figs/Table_S1_SquirrelInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Cecum_Microbes/figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{8388A2C0-75F8-4A0B-8067-DF38FB183ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{721BAEF6-8BEC-4125-8F44-0FBF20E60DC4}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{8388A2C0-75F8-4A0B-8067-DF38FB183ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E3AAB4E-A290-4C1E-A5CE-9F0A0971D1CF}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F729A4CA-F102-4347-A089-5DE75D0FF591}"/>
+    <workbookView xWindow="12255" yWindow="45" windowWidth="16260" windowHeight="14550" xr2:uid="{F729A4CA-F102-4347-A089-5DE75D0FF591}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="28">
   <si>
     <t>Sex</t>
   </si>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t>Age at Sampling (days)</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>059</t>
+  </si>
+  <si>
+    <t>060</t>
   </si>
 </sst>
 </file>
@@ -176,9 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,603 +511,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7E20A2-4090-4D21-B9BE-0070BCCDCA6A}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3881</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>881</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>185</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>34.1</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3882</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>882</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>160</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>34.4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3883</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>883</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>150</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>35</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3884</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>884</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
       <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>136</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>5.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3885</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>885</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
       <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>143</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4.5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3886</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>886</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
       <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>168</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4.2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3889</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>889</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
       <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>177</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>32.4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3890</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>890</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
       <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>167</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3894</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>894</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>154</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3895</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>895</v>
+      </c>
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
       <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>141</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>3.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3899</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>899</v>
+      </c>
+      <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>13</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>184</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3901</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>901</v>
+      </c>
+      <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>160</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>3.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3906</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>906</v>
+      </c>
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
       <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>141</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3907</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>907</v>
+      </c>
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
       <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>176</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>35.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3910</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>910</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
       <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>136</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3911</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>911</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>12</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>164</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3912</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>912</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>12</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>165</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>35.9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3916</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <v>916</v>
+      </c>
+      <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
       <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
         <v>12</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>122</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3917</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20">
+        <v>917</v>
+      </c>
+      <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
       <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
         <v>12</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>127</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3919</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <v>919</v>
+      </c>
+      <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>12</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>169</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>38.6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3920</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22">
+        <v>920</v>
+      </c>
+      <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>12</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>134</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>34.1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3921</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23">
+        <v>921</v>
+      </c>
+      <c r="C23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
       <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>158</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>37.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3922</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24">
+        <v>922</v>
+      </c>
+      <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>16</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>136</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3923</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25">
+        <v>923</v>
+      </c>
+      <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>8</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>15</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>170</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>33.9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3924</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26">
+        <v>924</v>
+      </c>
+      <c r="C26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
       <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
         <v>15</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>134</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3925</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27">
+        <v>925</v>
+      </c>
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
       <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
         <v>15</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>136</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4057</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
@@ -1097,19 +1197,22 @@
       <c r="F28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4058</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
@@ -1117,19 +1220,22 @@
       <c r="F29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4059</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
@@ -1137,24 +1243,30 @@
       <c r="F30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4060</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
         <v>9</v>
       </c>
       <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>